<commit_message>
code cleaning and reports.
</commit_message>
<xml_diff>
--- a/report/YearByYearEarthquakes.xlsx
+++ b/report/YearByYearEarthquakes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\alper_workspace\P2-hiep_alper_team\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\alper_workspace\P2-hiep_alper_team\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14550" windowHeight="6585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14550" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="YearByYear EarthQuakes" sheetId="1" r:id="rId1"/>
@@ -410,11 +410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1976400704"/>
-        <c:axId val="1976388736"/>
+        <c:axId val="-1798501072"/>
+        <c:axId val="-1798509232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1976400704"/>
+        <c:axId val="-1798501072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,7 +457,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1976388736"/>
+        <c:crossAx val="-1798509232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -465,7 +465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1976388736"/>
+        <c:axId val="-1798509232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,7 +501,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1976400704"/>
+        <c:crossAx val="-1798501072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -971,11 +971,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="22320800"/>
-        <c:axId val="22308288"/>
+        <c:axId val="-1798508144"/>
+        <c:axId val="-1798507600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22320800"/>
+        <c:axId val="-1798508144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,7 +1018,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22308288"/>
+        <c:crossAx val="-1798507600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1026,7 +1026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22308288"/>
+        <c:axId val="-1798507600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1062,7 +1062,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="22320800"/>
+        <c:crossAx val="-1798508144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1427,11 +1427,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1103920000"/>
-        <c:axId val="1103926528"/>
+        <c:axId val="-1800177344"/>
+        <c:axId val="-1800175712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1103920000"/>
+        <c:axId val="-1800177344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,7 +1474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1103926528"/>
+        <c:crossAx val="-1800175712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1482,7 +1482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1103926528"/>
+        <c:axId val="-1800175712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1518,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1103920000"/>
+        <c:crossAx val="-1800177344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3768,7 +3768,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>